<commit_message>
feat: Insertion Sort by Title
Sort after adding new composition
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
   <si>
     <t>Test</t>
   </si>
@@ -76,6 +76,36 @@
   </si>
   <si>
     <t>Notes2</t>
+  </si>
+  <si>
+    <t>Bach Cello Suite</t>
+  </si>
+  <si>
+    <t>Bach</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Essential Elements</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Hi, Mr. Kelly!</t>
+  </si>
+  <si>
+    <t>The Elements</t>
+  </si>
+  <si>
+    <t>Richard Meyer</t>
+  </si>
+  <si>
+    <t>Hal Leonard</t>
+  </si>
+  <si>
+    <t>Really cool piece!</t>
   </si>
 </sst>
 </file>
@@ -394,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +432,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -422,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -438,6 +468,46 @@
       </c>
       <c r="F2" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>